<commit_message>
Did my 3rd filtering attempt at source 1 (huge dataset). Had to edit and redo python script for filtered movies.
</commit_message>
<xml_diff>
--- a/movie-release-optimization/data/cleaned/xlsx/marvel_movies.xlsx
+++ b/movie-release-optimization/data/cleaned/xlsx/marvel_movies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitkat/project 0/Marvel-Analytics-by-KS/movie-release-optimization/data/cleaned/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitkat/github projects/Marvel-Analytics-by-KS/movie-release-optimization/data/cleaned/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{17E1E0A2-8209-CE46-BF29-7E519EAAE5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12786699-175B-0244-BE89-B24ACBB80725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="20" windowWidth="19220" windowHeight="21600" xr2:uid="{0EAFD10D-0BCC-FA4E-8446-8BA5CD0E0E58}"/>
   </bookViews>
@@ -224,10 +224,10 @@
     <t>budget</t>
   </si>
   <si>
-    <t>release date</t>
-  </si>
-  <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>release_date</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -717,7 +717,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -765,7 +765,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -785,7 +785,7 @@
   <autoFilter ref="A1:C38" xr:uid="{4F992C7A-5EAC-974A-A11F-B998F619FB8E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0DD13513-F771-024A-A1CD-D8CE8FBDEF89}" name="title"/>
-    <tableColumn id="2" xr3:uid="{CEC484DF-8126-B241-A1D6-6ADFACA33B11}" name="release date" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{CEC484DF-8126-B241-A1D6-6ADFACA33B11}" name="release_date" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{F27F467F-F2C5-3D4A-8EDA-9BEA1680320D}" name="budget"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,10 +1124,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>62</v>

</xml_diff>